<commit_message>
refactored tests to have only one xl snapshot per test
</commit_message>
<xml_diff>
--- a/tests/testthat/_snaps/knitxl/headers1.xlsx
+++ b/tests/testthat/_snaps/knitxl/headers1.xlsx
@@ -12,9 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t xml:space="preserve"># Header 1text## Header 2text### Header 3text#### Header 4text##### Header 5text###### Header 6text</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t xml:space="preserve">Header 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header 6</t>
   </si>
 </sst>
 </file>
@@ -22,7 +40,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -31,9 +49,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF475368"/>
+      <name val="Calibri Light (Headings)"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF475368"/>
+      <name val="Calibri (Body)"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF475368"/>
+      <name val="Calibri (Body)"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF475368"/>
+      <name val="Calibri (Body)"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF475368"/>
+      <name val="Calibri (Body)"/>
+      <i/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -52,13 +99,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FF4F71BE"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFA6B7DE"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium">
+        <color rgb="FFA6B7DE"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,6 +425,61 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>